<commit_message>
Ajout des assertions et modifications du sendmail
</commit_message>
<xml_diff>
--- a/src/test/resources/reports/Verification.xlsx
+++ b/src/test/resources/reports/Verification.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="59">
   <si>
     <t>Numero bug</t>
   </si>
@@ -182,6 +182,21 @@
   </si>
   <si>
     <t>17:51:40</t>
+  </si>
+  <si>
+    <t>2021-06-11</t>
+  </si>
+  <si>
+    <t>16:25:03</t>
+  </si>
+  <si>
+    <t>16:25:20</t>
+  </si>
+  <si>
+    <t>16:25:32</t>
+  </si>
+  <si>
+    <t>16:26:55</t>
   </si>
 </sst>
 </file>
@@ -351,7 +366,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="191">
+  <cellXfs count="199">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -373,6 +388,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
@@ -938,42 +961,42 @@
       <c r="A23" t="s">
         <v>5</v>
       </c>
-      <c r="B23" t="s" s="189">
+      <c r="B23" t="s" s="197">
         <v>9</v>
       </c>
       <c r="C23" t="s">
-        <v>7</v>
+        <v>54</v>
       </c>
       <c r="D23" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
         <v>14</v>
       </c>
-      <c r="B24" t="s" s="190">
+      <c r="B24" t="s" s="198">
         <v>6</v>
       </c>
       <c r="C24" t="s">
-        <v>7</v>
+        <v>54</v>
       </c>
       <c r="D24" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
         <v>48</v>
       </c>
-      <c r="B25" t="s" s="190">
+      <c r="B25" t="s" s="198">
         <v>6</v>
       </c>
       <c r="C25" t="s">
-        <v>7</v>
+        <v>54</v>
       </c>
       <c r="D25" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>